<commit_message>
Update Testcases 29-32 with smaller subject annotation file
</commit_message>
<xml_diff>
--- a/data/qa/QTP/Test029.xlsx
+++ b/data/qa/QTP/Test029.xlsx
@@ -195,9 +195,6 @@
     <t>Group Name=SUBJECTS, Description=subjects, File= https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Annotation_Groups/Annotation_Group.csv</t>
   </si>
   <si>
-    <t>Input filename= https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Subject_Data/Subject_Data.csv</t>
-  </si>
-  <si>
     <t>Input data from https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Genomic/Parsed/caArray_data_source_parsed_3samples.xls and click save</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Test029</t>
+  </si>
+  <si>
+    <t>Input filename= https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Subject_Data/Subject_Data-small3x3.csv</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -813,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
         <v>53</v>
@@ -835,10 +835,10 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" t="s">
         <v>62</v>
-      </c>
-      <c r="H18" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="6:9">
@@ -846,13 +846,13 @@
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="6:9">
@@ -860,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
         <v>54</v>
@@ -882,7 +882,7 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
         <v>42</v>

</xml_diff>